<commit_message>
1.9.1. Pre Final 2.
</commit_message>
<xml_diff>
--- a/Schedule Calculator Pro/bin/Debug/Вільні аудиторії.xlsx
+++ b/Schedule Calculator Pro/bin/Debug/Вільні аудиторії.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\SCP\Schedule Calculator Pro\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE36494-E830-46EB-A586-B75B0BFCFBA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E05A895-ED07-4548-9775-E045A7D5EF67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14475" yWindow="2805" windowWidth="13995" windowHeight="11505" xr2:uid="{9700FD65-07A4-429E-A4D8-FD4F24C0BB3D}"/>
+    <workbookView xWindow="14805" yWindow="1095" windowWidth="13995" windowHeight="11505" xr2:uid="{C989C8D2-CB96-4B23-8DDE-60F48638D997}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
   <si>
     <t>Перша пара</t>
   </si>
@@ -39,13 +33,10 @@
     <t>318/</t>
   </si>
   <si>
-    <t>111/</t>
+    <t>405/</t>
   </si>
   <si>
     <t>с.з.</t>
-  </si>
-  <si>
-    <t>311/</t>
   </si>
   <si>
     <t>Середа</t>
@@ -594,7 +585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58026389-1F19-4E5C-9AFB-2919C88B42AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2482C5C0-155B-4D77-87EF-6D14A9700755}">
   <dimension ref="A1:F296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -620,17 +611,17 @@
       <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="9">
         <v>104</v>
       </c>
       <c r="B2" s="6">
+        <v>108</v>
+      </c>
+      <c r="C2" s="9">
         <v>104</v>
       </c>
-      <c r="C2" s="9">
+      <c r="D2" s="9">
         <v>108</v>
-      </c>
-      <c r="D2" s="9">
-        <v>104</v>
       </c>
       <c r="E2" s="9">
         <v>104</v>
@@ -640,17 +631,17 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="9">
         <v>108</v>
       </c>
       <c r="B3" s="6">
+        <v>122</v>
+      </c>
+      <c r="C3" s="9">
         <v>108</v>
       </c>
-      <c r="C3" s="9">
+      <c r="D3" s="9">
         <v>112</v>
-      </c>
-      <c r="D3" s="9">
-        <v>105</v>
       </c>
       <c r="E3" s="9">
         <v>105</v>
@@ -660,17 +651,17 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="9">
         <v>112</v>
       </c>
       <c r="B4" s="6">
+        <v>123</v>
+      </c>
+      <c r="C4" s="9">
         <v>112</v>
       </c>
-      <c r="C4" s="9">
+      <c r="D4" s="9">
         <v>122</v>
-      </c>
-      <c r="D4" s="9">
-        <v>108</v>
       </c>
       <c r="E4" s="9">
         <v>106</v>
@@ -680,17 +671,17 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="9">
         <v>122</v>
       </c>
       <c r="B5" s="6">
+        <v>151</v>
+      </c>
+      <c r="C5" s="9">
         <v>122</v>
       </c>
-      <c r="C5" s="9">
-        <v>152</v>
-      </c>
       <c r="D5" s="9">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="E5" s="9">
         <v>108</v>
@@ -700,17 +691,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="9">
+        <v>152</v>
+      </c>
+      <c r="B6" s="6">
+        <v>152</v>
+      </c>
+      <c r="C6" s="9">
         <v>123</v>
       </c>
-      <c r="B6" s="6">
-        <v>123</v>
-      </c>
-      <c r="C6" s="9">
-        <v>153</v>
-      </c>
       <c r="D6" s="9">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="E6" s="9">
         <v>109</v>
@@ -720,17 +711,17 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="9">
+        <v>153</v>
+      </c>
+      <c r="B7" s="6">
+        <v>153</v>
+      </c>
+      <c r="C7" s="9">
         <v>151</v>
       </c>
-      <c r="B7" s="6">
-        <v>151</v>
-      </c>
-      <c r="C7" s="9">
-        <v>154</v>
-      </c>
       <c r="D7" s="9">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="E7" s="9">
         <v>111</v>
@@ -740,17 +731,17 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="9">
+        <v>154</v>
+      </c>
+      <c r="B8" s="6">
+        <v>202</v>
+      </c>
+      <c r="C8" s="9">
         <v>152</v>
       </c>
-      <c r="B8" s="6">
-        <v>152</v>
-      </c>
-      <c r="C8" s="9">
-        <v>201</v>
-      </c>
       <c r="D8" s="9">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="E8" s="9">
         <v>112</v>
@@ -760,17 +751,17 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>202</v>
+      <c r="A9" s="9">
+        <v>200</v>
       </c>
       <c r="B9" s="6">
+        <v>203</v>
+      </c>
+      <c r="C9" s="9">
         <v>153</v>
       </c>
-      <c r="C9" s="9">
-        <v>203</v>
-      </c>
       <c r="D9" s="9">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E9" s="9">
         <v>117</v>
@@ -780,17 +771,17 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>203</v>
+      <c r="A10" s="9">
+        <v>201</v>
       </c>
       <c r="B10" s="6">
+        <v>206</v>
+      </c>
+      <c r="C10" s="9">
         <v>154</v>
       </c>
-      <c r="C10" s="9">
-        <v>204</v>
-      </c>
       <c r="D10" s="9">
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="E10" s="9">
         <v>122</v>
@@ -800,17 +791,17 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>206</v>
+      <c r="A11" s="9">
+        <v>202</v>
       </c>
       <c r="B11" s="6">
+        <v>208</v>
+      </c>
+      <c r="C11" s="9">
         <v>200</v>
       </c>
-      <c r="C11" s="9">
-        <v>208</v>
-      </c>
       <c r="D11" s="9">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="E11" s="9">
         <v>123</v>
@@ -820,17 +811,17 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>208</v>
+      <c r="A12" s="9">
+        <v>204</v>
       </c>
       <c r="B12" s="6">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C12" s="9">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D12" s="9">
-        <v>154</v>
+        <v>203</v>
       </c>
       <c r="E12" s="9">
         <v>151</v>
@@ -840,17 +831,17 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="9">
+        <v>208</v>
+      </c>
+      <c r="B13" s="6">
         <v>210</v>
       </c>
-      <c r="B13" s="6">
-        <v>206</v>
-      </c>
       <c r="C13" s="9">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D13" s="9">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E13" s="9">
         <v>152</v>
@@ -860,17 +851,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="9">
+        <v>209</v>
+      </c>
+      <c r="B14" s="6">
         <v>211</v>
       </c>
-      <c r="B14" s="6">
-        <v>208</v>
-      </c>
       <c r="C14" s="9">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D14" s="9">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E14" s="9">
         <v>153</v>
@@ -880,17 +871,17 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>213</v>
+      <c r="A15" s="9">
+        <v>210</v>
       </c>
       <c r="B15" s="6">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C15" s="9">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D15" s="9">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="E15" s="9">
         <v>154</v>
@@ -900,17 +891,17 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>214</v>
+      <c r="A16" s="9">
+        <v>211</v>
       </c>
       <c r="B16" s="6">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C16" s="9">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D16" s="9">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="E16" s="9">
         <v>200</v>
@@ -920,17 +911,17 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>215</v>
+      <c r="A17" s="9">
+        <v>213</v>
       </c>
       <c r="B17" s="6">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C17" s="9">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D17" s="9">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E17" s="9">
         <v>201</v>
@@ -940,17 +931,17 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>216</v>
+      <c r="A18" s="9">
+        <v>215</v>
       </c>
       <c r="B18" s="6">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C18" s="9">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D18" s="9">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E18" s="9">
         <v>202</v>
@@ -960,17 +951,17 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>217</v>
+      <c r="A19" s="9">
+        <v>216</v>
       </c>
       <c r="B19" s="6">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C19" s="9">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D19" s="9">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E19" s="9">
         <v>203</v>
@@ -980,17 +971,17 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>218</v>
+      <c r="A20" s="9">
+        <v>217</v>
       </c>
       <c r="B20" s="6">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C20" s="9">
-        <v>304</v>
+        <v>215</v>
       </c>
       <c r="D20" s="9">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E20" s="9">
         <v>204</v>
@@ -1000,17 +991,17 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>219</v>
+      <c r="A21" s="9">
+        <v>218</v>
       </c>
       <c r="B21" s="6">
-        <v>219</v>
+        <v>304</v>
       </c>
       <c r="C21" s="9">
-        <v>306</v>
+        <v>216</v>
       </c>
       <c r="D21" s="9">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E21" s="9">
         <v>206</v>
@@ -1020,17 +1011,17 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>302</v>
+      <c r="A22" s="9">
+        <v>219</v>
       </c>
       <c r="B22" s="6">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C22" s="9">
-        <v>308</v>
+        <v>217</v>
       </c>
       <c r="D22" s="9">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E22" s="9">
         <v>208</v>
@@ -1040,17 +1031,17 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>303</v>
+      <c r="A23" s="9">
+        <v>302</v>
       </c>
       <c r="B23" s="6">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C23" s="9">
-        <v>310</v>
+        <v>218</v>
       </c>
       <c r="D23" s="9">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E23" s="9">
         <v>209</v>
@@ -1060,17 +1051,17 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>304</v>
+      <c r="A24" s="9">
+        <v>303</v>
       </c>
       <c r="B24" s="6">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C24" s="9">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="D24" s="9">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E24" s="9">
         <v>210</v>
@@ -1080,17 +1071,17 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>306</v>
+      <c r="A25" s="9">
+        <v>304</v>
       </c>
       <c r="B25" s="6">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C25" s="9">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="D25" s="9">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E25" s="9">
         <v>211</v>
@@ -1100,17 +1091,17 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>308</v>
+      <c r="A26" s="9">
+        <v>306</v>
       </c>
       <c r="B26" s="6">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C26" s="9">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="D26" s="9">
-        <v>217</v>
+        <v>301</v>
       </c>
       <c r="E26" s="9">
         <v>213</v>
@@ -1120,17 +1111,17 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>310</v>
+      <c r="A27" s="9">
+        <v>308</v>
       </c>
       <c r="B27" s="6">
         <v>321</v>
       </c>
       <c r="C27" s="9">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="D27" s="9">
-        <v>218</v>
+        <v>303</v>
       </c>
       <c r="E27" s="9">
         <v>214</v>
@@ -1140,17 +1131,17 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>314</v>
+      <c r="A28" s="9">
+        <v>310</v>
       </c>
       <c r="B28" s="6">
         <v>322</v>
       </c>
       <c r="C28" s="9">
-        <v>403</v>
+        <v>317</v>
       </c>
       <c r="D28" s="9">
-        <v>219</v>
+        <v>304</v>
       </c>
       <c r="E28" s="9">
         <v>215</v>
@@ -1160,17 +1151,17 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="A29" s="9">
         <v>317</v>
       </c>
       <c r="B29" s="6">
         <v>403</v>
       </c>
       <c r="C29" s="9">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D29" s="9">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="E29" s="9">
         <v>216</v>
@@ -1180,17 +1171,17 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="A30" s="9">
         <v>322</v>
       </c>
       <c r="B30" s="6">
         <v>404</v>
       </c>
       <c r="C30" s="9">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D30" s="9">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="E30" s="9">
         <v>217</v>
@@ -1200,17 +1191,17 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6">
+      <c r="A31" s="9">
+        <v>403</v>
+      </c>
+      <c r="B31" s="6">
+        <v>412</v>
+      </c>
+      <c r="C31" s="10">
         <v>405</v>
       </c>
-      <c r="B31" s="6">
-        <v>405</v>
-      </c>
-      <c r="C31" s="10">
-        <v>416</v>
-      </c>
       <c r="D31" s="9">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="E31" s="9">
         <v>218</v>
@@ -1219,15 +1210,15 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10">
+        <v>404</v>
+      </c>
+      <c r="B32" s="6">
         <v>416</v>
       </c>
-      <c r="B32" s="6">
-        <v>412</v>
-      </c>
       <c r="D32" s="9">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="E32" s="9">
         <v>219</v>
@@ -1236,15 +1227,12 @@
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="7">
-        <v>416</v>
-      </c>
       <c r="D33" s="9">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E33" s="9">
         <v>301</v>
@@ -1253,9 +1241,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D34" s="9">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E34" s="9">
         <v>302</v>
@@ -1264,9 +1255,9 @@
         <v>302</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D35" s="9">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E35" s="9">
         <v>303</v>
@@ -1275,9 +1266,9 @@
         <v>303</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D36" s="9">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E36" s="9">
         <v>304</v>
@@ -1286,9 +1277,9 @@
         <v>304</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D37" s="9">
-        <v>322</v>
+        <v>403</v>
       </c>
       <c r="E37" s="9">
         <v>305</v>
@@ -1297,7 +1288,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D38" s="9">
         <v>404</v>
       </c>
@@ -1308,7 +1299,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D39" s="9">
         <v>405</v>
       </c>
@@ -1319,7 +1310,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D40" s="9">
         <v>409</v>
       </c>
@@ -1330,9 +1321,9 @@
         <v>310</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D41" s="9">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E41" s="9">
         <v>311</v>
@@ -1341,8 +1332,8 @@
         <v>311</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D42" s="9">
+    <row r="42" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="10">
         <v>416</v>
       </c>
       <c r="E42" s="9">
@@ -1352,10 +1343,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="10" t="s">
-        <v>2</v>
-      </c>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E43" s="9">
         <v>317</v>
       </c>
@@ -1363,7 +1351,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E44" s="9">
         <v>319</v>
       </c>
@@ -1371,7 +1359,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E45" s="9">
         <v>321</v>
       </c>
@@ -1379,7 +1367,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E46" s="9">
         <v>322</v>
       </c>
@@ -1387,7 +1375,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E47" s="9">
         <v>403</v>
       </c>
@@ -1395,7 +1383,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E48" s="9">
         <v>404</v>
       </c>
@@ -1485,7 +1473,7 @@
       <c r="A60" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="8"/>
+      <c r="B60" s="5"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="5"/>
@@ -1495,8 +1483,8 @@
       <c r="A61" s="6">
         <v>104</v>
       </c>
-      <c r="B61" s="9">
-        <v>108</v>
+      <c r="B61" s="6">
+        <v>104</v>
       </c>
       <c r="C61" s="9">
         <v>104</v>
@@ -1513,10 +1501,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
-        <v>106</v>
-      </c>
-      <c r="B62" s="9">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="B62" s="6">
+        <v>108</v>
       </c>
       <c r="C62" s="9">
         <v>108</v>
@@ -1533,13 +1521,13 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
-        <v>108</v>
-      </c>
-      <c r="B63" s="9">
+        <v>112</v>
+      </c>
+      <c r="B63" s="6">
         <v>117</v>
       </c>
       <c r="C63" s="9">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D63" s="9">
         <v>106</v>
@@ -1553,13 +1541,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
+        <v>122</v>
+      </c>
+      <c r="B64" s="6">
+        <v>151</v>
+      </c>
+      <c r="C64" s="9">
         <v>112</v>
-      </c>
-      <c r="B64" s="9">
-        <v>122</v>
-      </c>
-      <c r="C64" s="9">
-        <v>117</v>
       </c>
       <c r="D64" s="9">
         <v>108</v>
@@ -1573,13 +1561,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
-        <v>122</v>
-      </c>
-      <c r="B65" s="9">
         <v>123</v>
       </c>
+      <c r="B65" s="6">
+        <v>153</v>
+      </c>
       <c r="C65" s="9">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D65" s="9">
         <v>109</v>
@@ -1593,13 +1581,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
-        <v>123</v>
-      </c>
-      <c r="B66" s="9">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="B66" s="6">
+        <v>154</v>
       </c>
       <c r="C66" s="9">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="D66" s="9">
         <v>111</v>
@@ -1613,16 +1601,16 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
+        <v>153</v>
+      </c>
+      <c r="B67" s="6">
+        <v>200</v>
+      </c>
+      <c r="C67" s="9">
         <v>151</v>
       </c>
-      <c r="B67" s="9">
-        <v>152</v>
-      </c>
-      <c r="C67" s="9">
-        <v>152</v>
-      </c>
       <c r="D67" s="9">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E67" s="6">
         <v>112</v>
@@ -1633,16 +1621,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
+        <v>154</v>
+      </c>
+      <c r="B68" s="6">
+        <v>201</v>
+      </c>
+      <c r="C68" s="9">
         <v>152</v>
       </c>
-      <c r="B68" s="9">
-        <v>153</v>
-      </c>
-      <c r="C68" s="9">
-        <v>153</v>
-      </c>
       <c r="D68" s="9">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E68" s="6">
         <v>117</v>
@@ -1653,16 +1641,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
-        <v>154</v>
-      </c>
-      <c r="B69" s="9">
-        <v>154</v>
+        <v>200</v>
+      </c>
+      <c r="B69" s="6">
+        <v>202</v>
       </c>
       <c r="C69" s="9">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D69" s="9">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E69" s="6">
         <v>122</v>
@@ -1673,16 +1661,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
-        <v>200</v>
-      </c>
-      <c r="B70" s="9">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="B70" s="6">
+        <v>203</v>
       </c>
       <c r="C70" s="9">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="D70" s="9">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="E70" s="6">
         <v>123</v>
@@ -1693,16 +1681,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
-        <v>201</v>
-      </c>
-      <c r="B71" s="9">
-        <v>201</v>
+        <v>203</v>
+      </c>
+      <c r="B71" s="6">
+        <v>204</v>
       </c>
       <c r="C71" s="9">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D71" s="9">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E71" s="6">
         <v>151</v>
@@ -1713,16 +1701,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
-        <v>202</v>
-      </c>
-      <c r="B72" s="9">
-        <v>203</v>
+        <v>204</v>
+      </c>
+      <c r="B72" s="6">
+        <v>206</v>
       </c>
       <c r="C72" s="9">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D72" s="9">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E72" s="6">
         <v>152</v>
@@ -1733,16 +1721,16 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
-        <v>203</v>
-      </c>
-      <c r="B73" s="9">
-        <v>204</v>
+        <v>206</v>
+      </c>
+      <c r="B73" s="6">
+        <v>209</v>
       </c>
       <c r="C73" s="9">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D73" s="9">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E73" s="6">
         <v>153</v>
@@ -1753,16 +1741,16 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
-        <v>204</v>
-      </c>
-      <c r="B74" s="9">
-        <v>209</v>
+        <v>208</v>
+      </c>
+      <c r="B74" s="6">
+        <v>210</v>
       </c>
       <c r="C74" s="9">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D74" s="9">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="E74" s="6">
         <v>154</v>
@@ -1773,16 +1761,16 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
-        <v>208</v>
-      </c>
-      <c r="B75" s="9">
-        <v>210</v>
+        <v>209</v>
+      </c>
+      <c r="B75" s="6">
+        <v>211</v>
       </c>
       <c r="C75" s="9">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D75" s="9">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E75" s="6">
         <v>200</v>
@@ -1795,14 +1783,14 @@
       <c r="A76" s="6">
         <v>210</v>
       </c>
-      <c r="B76" s="9">
-        <v>211</v>
+      <c r="B76" s="6">
+        <v>213</v>
       </c>
       <c r="C76" s="9">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D76" s="9">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E76" s="6">
         <v>201</v>
@@ -1813,16 +1801,16 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
-        <v>213</v>
-      </c>
-      <c r="B77" s="9">
-        <v>213</v>
+        <v>211</v>
+      </c>
+      <c r="B77" s="6">
+        <v>214</v>
       </c>
       <c r="C77" s="9">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D77" s="9">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E77" s="6">
         <v>202</v>
@@ -1835,14 +1823,14 @@
       <c r="A78" s="6">
         <v>214</v>
       </c>
-      <c r="B78" s="9">
-        <v>214</v>
+      <c r="B78" s="6">
+        <v>215</v>
       </c>
       <c r="C78" s="9">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D78" s="9">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E78" s="6">
         <v>203</v>
@@ -1853,16 +1841,16 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
-        <v>217</v>
-      </c>
-      <c r="B79" s="9">
-        <v>217</v>
+        <v>215</v>
+      </c>
+      <c r="B79" s="6">
+        <v>218</v>
       </c>
       <c r="C79" s="9">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D79" s="9">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E79" s="6">
         <v>204</v>
@@ -1873,16 +1861,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
-        <v>218</v>
-      </c>
-      <c r="B80" s="9">
-        <v>218</v>
+        <v>216</v>
+      </c>
+      <c r="B80" s="6">
+        <v>219</v>
       </c>
       <c r="C80" s="9">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D80" s="9">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E80" s="6">
         <v>206</v>
@@ -1893,16 +1881,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
-        <v>219</v>
-      </c>
-      <c r="B81" s="9">
-        <v>219</v>
+        <v>217</v>
+      </c>
+      <c r="B81" s="6">
+        <v>303</v>
       </c>
       <c r="C81" s="9">
-        <v>219</v>
+        <v>303</v>
       </c>
       <c r="D81" s="9">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E81" s="6">
         <v>208</v>
@@ -1913,16 +1901,16 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
-        <v>303</v>
-      </c>
-      <c r="B82" s="9">
-        <v>303</v>
+        <v>218</v>
+      </c>
+      <c r="B82" s="6">
+        <v>304</v>
       </c>
       <c r="C82" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D82" s="9">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E82" s="6">
         <v>209</v>
@@ -1933,16 +1921,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
-        <v>304</v>
-      </c>
-      <c r="B83" s="9">
-        <v>304</v>
+        <v>219</v>
+      </c>
+      <c r="B83" s="6">
+        <v>306</v>
       </c>
       <c r="C83" s="9">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D83" s="9">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E83" s="6">
         <v>210</v>
@@ -1953,16 +1941,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
-        <v>306</v>
-      </c>
-      <c r="B84" s="9">
-        <v>306</v>
+        <v>303</v>
+      </c>
+      <c r="B84" s="6">
+        <v>308</v>
       </c>
       <c r="C84" s="9">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D84" s="9">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E84" s="6">
         <v>211</v>
@@ -1973,16 +1961,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
-        <v>308</v>
-      </c>
-      <c r="B85" s="9">
+        <v>306</v>
+      </c>
+      <c r="B85" s="6">
         <v>310</v>
       </c>
       <c r="C85" s="9">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D85" s="9">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E85" s="6">
         <v>213</v>
@@ -1993,16 +1981,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
-        <v>310</v>
-      </c>
-      <c r="B86" s="9">
-        <v>317</v>
+        <v>308</v>
+      </c>
+      <c r="B86" s="6">
+        <v>314</v>
       </c>
       <c r="C86" s="9">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D86" s="9">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E86" s="6">
         <v>214</v>
@@ -2013,16 +2001,16 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
-        <v>314</v>
-      </c>
-      <c r="B87" s="9">
-        <v>321</v>
+        <v>310</v>
+      </c>
+      <c r="B87" s="6">
+        <v>317</v>
       </c>
       <c r="C87" s="9">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D87" s="9">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E87" s="6">
         <v>215</v>
@@ -2033,16 +2021,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
-        <v>317</v>
-      </c>
-      <c r="B88" s="9">
-        <v>322</v>
+        <v>314</v>
+      </c>
+      <c r="B88" s="6">
+        <v>321</v>
       </c>
       <c r="C88" s="9">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D88" s="9">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E88" s="6">
         <v>216</v>
@@ -2055,14 +2043,14 @@
       <c r="A89" s="6">
         <v>321</v>
       </c>
-      <c r="B89" s="9">
-        <v>403</v>
+      <c r="B89" s="6">
+        <v>322</v>
       </c>
       <c r="C89" s="9">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D89" s="9">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E89" s="6">
         <v>217</v>
@@ -2073,16 +2061,16 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
+        <v>322</v>
+      </c>
+      <c r="B90" s="6">
         <v>403</v>
       </c>
-      <c r="B90" s="9">
-        <v>405</v>
-      </c>
       <c r="C90" s="9">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D90" s="9">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E90" s="6">
         <v>218</v>
@@ -2093,16 +2081,16 @@
     </row>
     <row r="91" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
-        <v>404</v>
-      </c>
-      <c r="B91" s="10">
-        <v>416</v>
-      </c>
-      <c r="C91" s="9">
-        <v>404</v>
+        <v>403</v>
+      </c>
+      <c r="B91" s="7">
+        <v>405</v>
+      </c>
+      <c r="C91" s="10">
+        <v>405</v>
       </c>
       <c r="D91" s="9">
-        <v>219</v>
+        <v>301</v>
       </c>
       <c r="E91" s="6">
         <v>219</v>
@@ -2112,14 +2100,11 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="7">
-        <v>405</v>
-      </c>
-      <c r="C92" s="9">
-        <v>416</v>
+      <c r="A92" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="D92" s="9">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E92" s="6">
         <v>301</v>
@@ -2129,9 +2114,6 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C93" s="9">
-        <v>717</v>
-      </c>
       <c r="D93" s="9">
         <v>303</v>
       </c>
@@ -2142,10 +2124,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C94" s="10" t="s">
-        <v>4</v>
-      </c>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D94" s="9">
         <v>304</v>
       </c>
@@ -2323,7 +2302,7 @@
     </row>
     <row r="110" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D110" s="9">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E110" s="6">
         <v>409</v>
@@ -2334,7 +2313,7 @@
     </row>
     <row r="111" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D111" s="9">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E111" s="6">
         <v>410</v>
@@ -2345,7 +2324,7 @@
     </row>
     <row r="112" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D112" s="9">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E112" s="6">
         <v>411</v>
@@ -2356,7 +2335,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D113" s="9">
-        <v>717</v>
+        <v>416</v>
       </c>
       <c r="E113" s="6">
         <v>412</v>
@@ -2403,7 +2382,7 @@
     <row r="118" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="119" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2412,34 +2391,34 @@
       <c r="F119" s="3"/>
     </row>
     <row r="120" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="13" t="s">
+      <c r="A120" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B120" s="12" t="s">
+      <c r="B120" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C120" s="13" t="s">
+      <c r="D120" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D120" s="13" t="s">
-        <v>8</v>
-      </c>
       <c r="E120" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F120" s="12" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="9">
+      <c r="A121" s="6">
+        <v>105</v>
+      </c>
+      <c r="B121" s="9">
+        <v>104</v>
+      </c>
+      <c r="C121" s="9">
         <v>108</v>
-      </c>
-      <c r="B121" s="6">
-        <v>104</v>
-      </c>
-      <c r="C121" s="9">
-        <v>105</v>
       </c>
       <c r="D121" s="9">
         <v>104</v>
@@ -2452,11 +2431,11 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="9">
-        <v>112</v>
-      </c>
-      <c r="B122" s="6">
-        <v>105</v>
+      <c r="A122" s="6">
+        <v>106</v>
+      </c>
+      <c r="B122" s="9">
+        <v>108</v>
       </c>
       <c r="C122" s="9">
         <v>112</v>
@@ -2472,17 +2451,17 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="9">
-        <v>122</v>
-      </c>
-      <c r="B123" s="6">
-        <v>106</v>
+      <c r="A123" s="6">
+        <v>117</v>
+      </c>
+      <c r="B123" s="9">
+        <v>112</v>
       </c>
       <c r="C123" s="9">
         <v>122</v>
       </c>
       <c r="D123" s="9">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E123" s="9">
         <v>106</v>
@@ -2492,14 +2471,14 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="9">
+      <c r="A124" s="6">
         <v>123</v>
       </c>
-      <c r="B124" s="6">
-        <v>108</v>
+      <c r="B124" s="9">
+        <v>117</v>
       </c>
       <c r="C124" s="9">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="D124" s="9">
         <v>112</v>
@@ -2512,14 +2491,14 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="9">
+      <c r="A125" s="6">
         <v>152</v>
       </c>
-      <c r="B125" s="6">
-        <v>112</v>
+      <c r="B125" s="9">
+        <v>122</v>
       </c>
       <c r="C125" s="9">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D125" s="9">
         <v>117</v>
@@ -2532,14 +2511,14 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="9">
-        <v>154</v>
-      </c>
-      <c r="B126" s="6">
-        <v>117</v>
+      <c r="A126" s="6">
+        <v>153</v>
+      </c>
+      <c r="B126" s="9">
+        <v>123</v>
       </c>
       <c r="C126" s="9">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D126" s="9">
         <v>122</v>
@@ -2552,17 +2531,17 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="9">
-        <v>200</v>
-      </c>
-      <c r="B127" s="6">
+      <c r="A127" s="6">
+        <v>154</v>
+      </c>
+      <c r="B127" s="9">
         <v>151</v>
       </c>
       <c r="C127" s="9">
-        <v>200</v>
+        <v>153</v>
       </c>
       <c r="D127" s="9">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E127" s="9">
         <v>112</v>
@@ -2572,17 +2551,17 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="9">
+      <c r="A128" s="6">
         <v>201</v>
       </c>
-      <c r="B128" s="6">
+      <c r="B128" s="9">
         <v>152</v>
       </c>
       <c r="C128" s="9">
-        <v>201</v>
+        <v>154</v>
       </c>
       <c r="D128" s="9">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E128" s="9">
         <v>117</v>
@@ -2592,17 +2571,17 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="9">
+      <c r="A129" s="6">
         <v>202</v>
       </c>
-      <c r="B129" s="6">
+      <c r="B129" s="9">
+        <v>153</v>
+      </c>
+      <c r="C129" s="9">
         <v>200</v>
       </c>
-      <c r="C129" s="9">
-        <v>202</v>
-      </c>
       <c r="D129" s="9">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E129" s="9">
         <v>122</v>
@@ -2612,17 +2591,17 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="9">
+      <c r="A130" s="6">
         <v>203</v>
       </c>
-      <c r="B130" s="6">
+      <c r="B130" s="9">
+        <v>200</v>
+      </c>
+      <c r="C130" s="9">
         <v>201</v>
       </c>
-      <c r="C130" s="9">
-        <v>203</v>
-      </c>
       <c r="D130" s="9">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E130" s="9">
         <v>123</v>
@@ -2632,17 +2611,17 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="9">
+      <c r="A131" s="6">
         <v>204</v>
       </c>
-      <c r="B131" s="6">
+      <c r="B131" s="9">
+        <v>201</v>
+      </c>
+      <c r="C131" s="9">
         <v>202</v>
       </c>
-      <c r="C131" s="9">
-        <v>204</v>
-      </c>
       <c r="D131" s="9">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="E131" s="9">
         <v>151</v>
@@ -2652,17 +2631,17 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="9">
+      <c r="A132" s="6">
         <v>206</v>
       </c>
-      <c r="B132" s="6">
+      <c r="B132" s="9">
         <v>203</v>
       </c>
       <c r="C132" s="9">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D132" s="9">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E132" s="9">
         <v>152</v>
@@ -2672,17 +2651,17 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="9">
+      <c r="A133" s="6">
         <v>208</v>
       </c>
-      <c r="B133" s="6">
+      <c r="B133" s="9">
         <v>204</v>
       </c>
       <c r="C133" s="9">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D133" s="9">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E133" s="9">
         <v>153</v>
@@ -2692,17 +2671,17 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="9">
+      <c r="A134" s="6">
         <v>209</v>
       </c>
-      <c r="B134" s="6">
+      <c r="B134" s="9">
         <v>206</v>
       </c>
       <c r="C134" s="9">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D134" s="9">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E134" s="9">
         <v>154</v>
@@ -2712,17 +2691,17 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="9">
-        <v>213</v>
-      </c>
-      <c r="B135" s="6">
-        <v>208</v>
+      <c r="A135" s="6">
+        <v>210</v>
+      </c>
+      <c r="B135" s="9">
+        <v>209</v>
       </c>
       <c r="C135" s="9">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D135" s="9">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E135" s="9">
         <v>200</v>
@@ -2732,17 +2711,17 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="9">
-        <v>214</v>
-      </c>
-      <c r="B136" s="6">
-        <v>209</v>
+      <c r="A136" s="6">
+        <v>213</v>
+      </c>
+      <c r="B136" s="9">
+        <v>210</v>
       </c>
       <c r="C136" s="9">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D136" s="9">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E136" s="9">
         <v>201</v>
@@ -2752,17 +2731,17 @@
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="9">
-        <v>215</v>
-      </c>
-      <c r="B137" s="6">
-        <v>213</v>
+      <c r="A137" s="6">
+        <v>216</v>
+      </c>
+      <c r="B137" s="9">
+        <v>211</v>
       </c>
       <c r="C137" s="9">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D137" s="9">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E137" s="9">
         <v>202</v>
@@ -2772,17 +2751,17 @@
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="9">
-        <v>216</v>
-      </c>
-      <c r="B138" s="6">
+      <c r="A138" s="6">
+        <v>217</v>
+      </c>
+      <c r="B138" s="9">
         <v>214</v>
       </c>
       <c r="C138" s="9">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D138" s="9">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E138" s="9">
         <v>203</v>
@@ -2792,17 +2771,17 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="9">
-        <v>217</v>
-      </c>
-      <c r="B139" s="6">
-        <v>216</v>
+      <c r="A139" s="6">
+        <v>219</v>
+      </c>
+      <c r="B139" s="9">
+        <v>215</v>
       </c>
       <c r="C139" s="9">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D139" s="9">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E139" s="9">
         <v>204</v>
@@ -2812,17 +2791,17 @@
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="9">
-        <v>218</v>
-      </c>
-      <c r="B140" s="6">
-        <v>217</v>
+      <c r="A140" s="6">
+        <v>303</v>
+      </c>
+      <c r="B140" s="9">
+        <v>216</v>
       </c>
       <c r="C140" s="9">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D140" s="9">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E140" s="9">
         <v>206</v>
@@ -2832,17 +2811,17 @@
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="9">
-        <v>219</v>
-      </c>
-      <c r="B141" s="6">
-        <v>218</v>
+      <c r="A141" s="6">
+        <v>304</v>
+      </c>
+      <c r="B141" s="9">
+        <v>217</v>
       </c>
       <c r="C141" s="9">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D141" s="9">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E141" s="9">
         <v>208</v>
@@ -2852,17 +2831,17 @@
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="9">
-        <v>303</v>
-      </c>
-      <c r="B142" s="6">
-        <v>302</v>
+      <c r="A142" s="6">
+        <v>306</v>
+      </c>
+      <c r="B142" s="9">
+        <v>218</v>
       </c>
       <c r="C142" s="9">
-        <v>302</v>
+        <v>218</v>
       </c>
       <c r="D142" s="9">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E142" s="9">
         <v>209</v>
@@ -2872,17 +2851,17 @@
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="9">
-        <v>306</v>
-      </c>
-      <c r="B143" s="6">
-        <v>304</v>
+      <c r="A143" s="6">
+        <v>308</v>
+      </c>
+      <c r="B143" s="9">
+        <v>303</v>
       </c>
       <c r="C143" s="9">
-        <v>303</v>
+        <v>219</v>
       </c>
       <c r="D143" s="9">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E143" s="9">
         <v>210</v>
@@ -2892,17 +2871,17 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="9">
-        <v>308</v>
-      </c>
-      <c r="B144" s="6">
-        <v>305</v>
+      <c r="A144" s="6">
+        <v>310</v>
+      </c>
+      <c r="B144" s="9">
+        <v>304</v>
       </c>
       <c r="C144" s="9">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D144" s="9">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E144" s="9">
         <v>211</v>
@@ -2912,17 +2891,17 @@
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="9">
-        <v>310</v>
-      </c>
-      <c r="B145" s="6">
-        <v>306</v>
+      <c r="A145" s="6">
+        <v>314</v>
+      </c>
+      <c r="B145" s="9">
+        <v>308</v>
       </c>
       <c r="C145" s="9">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D145" s="9">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E145" s="9">
         <v>213</v>
@@ -2932,14 +2911,14 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="9">
-        <v>314</v>
-      </c>
-      <c r="B146" s="6">
-        <v>308</v>
+      <c r="A146" s="6">
+        <v>317</v>
+      </c>
+      <c r="B146" s="9">
+        <v>311</v>
       </c>
       <c r="C146" s="9">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D146" s="9">
         <v>219</v>
@@ -2952,14 +2931,14 @@
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="9">
-        <v>317</v>
-      </c>
-      <c r="B147" s="6">
-        <v>310</v>
+      <c r="A147" s="6">
+        <v>321</v>
+      </c>
+      <c r="B147" s="9">
+        <v>314</v>
       </c>
       <c r="C147" s="9">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D147" s="9">
         <v>301</v>
@@ -2972,14 +2951,14 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="9">
+      <c r="A148" s="6">
         <v>322</v>
       </c>
-      <c r="B148" s="6">
+      <c r="B148" s="9">
+        <v>322</v>
+      </c>
+      <c r="C148" s="9">
         <v>311</v>
-      </c>
-      <c r="C148" s="9">
-        <v>317</v>
       </c>
       <c r="D148" s="9">
         <v>302</v>
@@ -2992,17 +2971,17 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="9">
-        <v>404</v>
-      </c>
-      <c r="B149" s="6">
+      <c r="A149" s="6">
+        <v>403</v>
+      </c>
+      <c r="B149" s="9">
+        <v>403</v>
+      </c>
+      <c r="C149" s="9">
         <v>314</v>
       </c>
-      <c r="C149" s="9">
-        <v>322</v>
-      </c>
       <c r="D149" s="9">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E149" s="9">
         <v>217</v>
@@ -3012,17 +2991,17 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="9">
-        <v>409</v>
-      </c>
-      <c r="B150" s="6">
+      <c r="A150" s="6">
+        <v>404</v>
+      </c>
+      <c r="B150" s="9">
+        <v>404</v>
+      </c>
+      <c r="C150" s="9">
         <v>317</v>
       </c>
-      <c r="C150" s="9">
-        <v>403</v>
-      </c>
       <c r="D150" s="9">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E150" s="9">
         <v>218</v>
@@ -3032,17 +3011,17 @@
       </c>
     </row>
     <row r="151" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="10">
-        <v>413</v>
-      </c>
-      <c r="B151" s="6">
+      <c r="A151" s="7">
+        <v>409</v>
+      </c>
+      <c r="B151" s="10">
+        <v>405</v>
+      </c>
+      <c r="C151" s="9">
         <v>321</v>
       </c>
-      <c r="C151" s="10">
-        <v>404</v>
-      </c>
       <c r="D151" s="9">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="E151" s="9">
         <v>219</v>
@@ -3052,11 +3031,11 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B152" s="6">
-        <v>322</v>
+      <c r="C152" s="9">
+        <v>403</v>
       </c>
       <c r="D152" s="9">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="E152" s="9">
         <v>301</v>
@@ -3065,12 +3044,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B153" s="6">
-        <v>403</v>
+    <row r="153" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C153" s="10">
+        <v>404</v>
       </c>
       <c r="D153" s="9">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E153" s="9">
         <v>302</v>
@@ -3079,12 +3058,9 @@
         <v>302</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="7">
-        <v>412</v>
-      </c>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D154" s="9">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E154" s="9">
         <v>303</v>
@@ -3095,7 +3071,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D155" s="9">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E155" s="9">
         <v>304</v>
@@ -3106,7 +3082,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D156" s="9">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E156" s="9">
         <v>305</v>
@@ -3117,7 +3093,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D157" s="9">
-        <v>322</v>
+        <v>403</v>
       </c>
       <c r="E157" s="9">
         <v>306</v>
@@ -3128,7 +3104,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" s="9">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E158" s="9">
         <v>308</v>
@@ -3139,7 +3115,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D159" s="9">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E159" s="9">
         <v>310</v>
@@ -3150,7 +3126,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D160" s="9">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="E160" s="9">
         <v>311</v>
@@ -3205,7 +3181,7 @@
     </row>
     <row r="165" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D165" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E165" s="9">
         <v>322</v>
@@ -3312,7 +3288,7 @@
       <c r="A179" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B179" s="8"/>
+      <c r="B179" s="5"/>
       <c r="C179" s="8"/>
       <c r="D179" s="8"/>
       <c r="E179" s="5"/>
@@ -3320,10 +3296,10 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="6">
-        <v>122</v>
-      </c>
-      <c r="B180" s="9">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="B180" s="6">
+        <v>109</v>
       </c>
       <c r="C180" s="9">
         <v>106</v>
@@ -3340,13 +3316,13 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="6">
-        <v>151</v>
-      </c>
-      <c r="B181" s="9">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="B181" s="6">
+        <v>112</v>
       </c>
       <c r="C181" s="9">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D181" s="9">
         <v>106</v>
@@ -3360,13 +3336,13 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="6">
-        <v>152</v>
-      </c>
-      <c r="B182" s="9">
+        <v>122</v>
+      </c>
+      <c r="B182" s="6">
+        <v>122</v>
+      </c>
+      <c r="C182" s="9">
         <v>112</v>
-      </c>
-      <c r="C182" s="9">
-        <v>122</v>
       </c>
       <c r="D182" s="9">
         <v>108</v>
@@ -3380,16 +3356,16 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="6">
-        <v>153</v>
-      </c>
-      <c r="B183" s="9">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="B183" s="6">
+        <v>123</v>
       </c>
       <c r="C183" s="9">
         <v>123</v>
       </c>
       <c r="D183" s="9">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E183" s="6">
         <v>108</v>
@@ -3400,16 +3376,16 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="6">
-        <v>154</v>
-      </c>
-      <c r="B184" s="9">
+        <v>151</v>
+      </c>
+      <c r="B184" s="6">
         <v>151</v>
       </c>
       <c r="C184" s="9">
         <v>151</v>
       </c>
       <c r="D184" s="9">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E184" s="6">
         <v>109</v>
@@ -3420,16 +3396,16 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="6">
-        <v>200</v>
-      </c>
-      <c r="B185" s="9">
+        <v>153</v>
+      </c>
+      <c r="B185" s="6">
         <v>152</v>
       </c>
       <c r="C185" s="9">
         <v>152</v>
       </c>
       <c r="D185" s="9">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E185" s="6">
         <v>111</v>
@@ -3440,16 +3416,16 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="6">
-        <v>201</v>
-      </c>
-      <c r="B186" s="9">
+        <v>154</v>
+      </c>
+      <c r="B186" s="6">
         <v>153</v>
       </c>
       <c r="C186" s="9">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D186" s="9">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E186" s="6">
         <v>112</v>
@@ -3460,16 +3436,16 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="6">
-        <v>202</v>
-      </c>
-      <c r="B187" s="9">
+        <v>200</v>
+      </c>
+      <c r="B187" s="6">
         <v>154</v>
       </c>
       <c r="C187" s="9">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="D187" s="9">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E187" s="6">
         <v>117</v>
@@ -3480,16 +3456,16 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="6">
-        <v>204</v>
-      </c>
-      <c r="B188" s="9">
         <v>201</v>
       </c>
+      <c r="B188" s="6">
+        <v>200</v>
+      </c>
       <c r="C188" s="9">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D188" s="9">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="E188" s="6">
         <v>122</v>
@@ -3500,16 +3476,16 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="6">
-        <v>208</v>
-      </c>
-      <c r="B189" s="9">
         <v>202</v>
       </c>
+      <c r="B189" s="6">
+        <v>201</v>
+      </c>
       <c r="C189" s="9">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D189" s="9">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E189" s="6">
         <v>123</v>
@@ -3520,16 +3496,16 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="6">
-        <v>209</v>
-      </c>
-      <c r="B190" s="9">
         <v>203</v>
       </c>
+      <c r="B190" s="6">
+        <v>202</v>
+      </c>
       <c r="C190" s="9">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D190" s="9">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E190" s="6">
         <v>151</v>
@@ -3540,16 +3516,16 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="6">
-        <v>210</v>
-      </c>
-      <c r="B191" s="9">
         <v>204</v>
       </c>
+      <c r="B191" s="6">
+        <v>204</v>
+      </c>
       <c r="C191" s="9">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D191" s="9">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E191" s="6">
         <v>152</v>
@@ -3560,16 +3536,16 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="6">
-        <v>211</v>
-      </c>
-      <c r="B192" s="9">
         <v>206</v>
       </c>
+      <c r="B192" s="6">
+        <v>206</v>
+      </c>
       <c r="C192" s="9">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D192" s="9">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="E192" s="6">
         <v>153</v>
@@ -3580,16 +3556,16 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="6">
-        <v>214</v>
-      </c>
-      <c r="B193" s="9">
         <v>208</v>
       </c>
+      <c r="B193" s="6">
+        <v>208</v>
+      </c>
       <c r="C193" s="9">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D193" s="9">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E193" s="6">
         <v>154</v>
@@ -3600,16 +3576,16 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="6">
-        <v>215</v>
-      </c>
-      <c r="B194" s="9">
         <v>209</v>
       </c>
+      <c r="B194" s="6">
+        <v>210</v>
+      </c>
       <c r="C194" s="9">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D194" s="9">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E194" s="6">
         <v>200</v>
@@ -3620,16 +3596,16 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="6">
-        <v>216</v>
-      </c>
-      <c r="B195" s="9">
         <v>210</v>
       </c>
+      <c r="B195" s="6">
+        <v>213</v>
+      </c>
       <c r="C195" s="9">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D195" s="9">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E195" s="6">
         <v>201</v>
@@ -3640,16 +3616,16 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="6">
-        <v>217</v>
-      </c>
-      <c r="B196" s="9">
-        <v>211</v>
+        <v>213</v>
+      </c>
+      <c r="B196" s="6">
+        <v>215</v>
       </c>
       <c r="C196" s="9">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D196" s="9">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E196" s="6">
         <v>202</v>
@@ -3660,16 +3636,16 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="6">
-        <v>218</v>
-      </c>
-      <c r="B197" s="9">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="B197" s="6">
+        <v>216</v>
       </c>
       <c r="C197" s="9">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D197" s="9">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E197" s="6">
         <v>203</v>
@@ -3680,16 +3656,16 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="6">
-        <v>219</v>
-      </c>
-      <c r="B198" s="9">
-        <v>214</v>
+        <v>216</v>
+      </c>
+      <c r="B198" s="6">
+        <v>217</v>
       </c>
       <c r="C198" s="9">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D198" s="9">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E198" s="6">
         <v>204</v>
@@ -3700,16 +3676,16 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="6">
-        <v>303</v>
-      </c>
-      <c r="B199" s="9">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="B199" s="6">
+        <v>218</v>
       </c>
       <c r="C199" s="9">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D199" s="9">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E199" s="6">
         <v>206</v>
@@ -3720,16 +3696,16 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="6">
-        <v>304</v>
-      </c>
-      <c r="B200" s="9">
-        <v>216</v>
+        <v>218</v>
+      </c>
+      <c r="B200" s="6">
+        <v>219</v>
       </c>
       <c r="C200" s="9">
-        <v>303</v>
+        <v>219</v>
       </c>
       <c r="D200" s="9">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E200" s="6">
         <v>208</v>
@@ -3740,16 +3716,16 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="6">
-        <v>305</v>
-      </c>
-      <c r="B201" s="9">
-        <v>217</v>
+        <v>219</v>
+      </c>
+      <c r="B201" s="6">
+        <v>304</v>
       </c>
       <c r="C201" s="9">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D201" s="9">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E201" s="6">
         <v>209</v>
@@ -3760,16 +3736,16 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="6">
+        <v>303</v>
+      </c>
+      <c r="B202" s="6">
         <v>306</v>
       </c>
-      <c r="B202" s="9">
-        <v>219</v>
-      </c>
       <c r="C202" s="9">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D202" s="9">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E202" s="6">
         <v>210</v>
@@ -3780,16 +3756,16 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="6">
+        <v>304</v>
+      </c>
+      <c r="B203" s="6">
         <v>308</v>
       </c>
-      <c r="B203" s="9">
-        <v>303</v>
-      </c>
       <c r="C203" s="9">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D203" s="9">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E203" s="6">
         <v>211</v>
@@ -3800,16 +3776,16 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="6">
-        <v>314</v>
-      </c>
-      <c r="B204" s="9">
-        <v>304</v>
+        <v>305</v>
+      </c>
+      <c r="B204" s="6">
+        <v>310</v>
       </c>
       <c r="C204" s="9">
         <v>308</v>
       </c>
       <c r="D204" s="9">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E204" s="6">
         <v>213</v>
@@ -3820,16 +3796,16 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="6">
-        <v>317</v>
-      </c>
-      <c r="B205" s="9">
         <v>306</v>
+      </c>
+      <c r="B205" s="6">
+        <v>314</v>
       </c>
       <c r="C205" s="9">
         <v>310</v>
       </c>
       <c r="D205" s="9">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E205" s="6">
         <v>214</v>
@@ -3840,16 +3816,16 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="6">
-        <v>318</v>
-      </c>
-      <c r="B206" s="9">
         <v>308</v>
       </c>
+      <c r="B206" s="6">
+        <v>317</v>
+      </c>
       <c r="C206" s="9">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D206" s="9">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E206" s="6">
         <v>215</v>
@@ -3860,16 +3836,16 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="6">
-        <v>321</v>
-      </c>
-      <c r="B207" s="9">
-        <v>311</v>
+        <v>310</v>
+      </c>
+      <c r="B207" s="6">
+        <v>318</v>
       </c>
       <c r="C207" s="9">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D207" s="9">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E207" s="6">
         <v>216</v>
@@ -3880,16 +3856,16 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="6">
-        <v>322</v>
-      </c>
-      <c r="B208" s="9">
         <v>314</v>
       </c>
+      <c r="B208" s="6">
+        <v>319</v>
+      </c>
       <c r="C208" s="9">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D208" s="9">
-        <v>219</v>
+        <v>301</v>
       </c>
       <c r="E208" s="6">
         <v>217</v>
@@ -3900,16 +3876,16 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="6">
-        <v>404</v>
-      </c>
-      <c r="B209" s="9">
         <v>321</v>
       </c>
+      <c r="B209" s="6">
+        <v>321</v>
+      </c>
       <c r="C209" s="9">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D209" s="9">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E209" s="6">
         <v>218</v>
@@ -3920,16 +3896,16 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="6">
-        <v>405</v>
-      </c>
-      <c r="B210" s="9">
-        <v>404</v>
+        <v>322</v>
+      </c>
+      <c r="B210" s="6">
+        <v>322</v>
       </c>
       <c r="C210" s="9">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D210" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E210" s="6">
         <v>219</v>
@@ -3938,18 +3914,18 @@
         <v>219</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="7">
-        <v>413</v>
-      </c>
-      <c r="B211" s="10">
-        <v>413</v>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="6">
+        <v>403</v>
+      </c>
+      <c r="B211" s="6">
+        <v>403</v>
       </c>
       <c r="C211" s="9">
-        <v>322</v>
+        <v>403</v>
       </c>
       <c r="D211" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E211" s="6">
         <v>301</v>
@@ -3959,11 +3935,17 @@
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="6">
+        <v>404</v>
+      </c>
+      <c r="B212" s="6">
+        <v>404</v>
+      </c>
       <c r="C212" s="9">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D212" s="9">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E212" s="6">
         <v>302</v>
@@ -3972,12 +3954,18 @@
         <v>302</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C213" s="9">
-        <v>404</v>
+    <row r="213" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="7">
+        <v>416</v>
+      </c>
+      <c r="B213" s="7">
+        <v>413</v>
+      </c>
+      <c r="C213" s="10">
+        <v>410</v>
       </c>
       <c r="D213" s="9">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E213" s="6">
         <v>303</v>
@@ -3986,12 +3974,9 @@
         <v>303</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C214" s="10">
-        <v>410</v>
-      </c>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D214" s="9">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E214" s="6">
         <v>304</v>
@@ -4002,7 +3987,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D215" s="9">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E215" s="6">
         <v>305</v>
@@ -4013,7 +3998,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D216" s="9">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E216" s="6">
         <v>306</v>
@@ -4024,7 +4009,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D217" s="9">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E217" s="6">
         <v>308</v>
@@ -4035,7 +4020,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D218" s="9">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E218" s="6">
         <v>310</v>
@@ -4046,7 +4031,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D219" s="9">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E219" s="6">
         <v>311</v>
@@ -4057,7 +4042,7 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D220" s="9">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E220" s="6">
         <v>314</v>
@@ -4068,7 +4053,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D221" s="9">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E221" s="6">
         <v>317</v>
@@ -4101,7 +4086,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D224" s="9">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="E224" s="6">
         <v>321</v>
@@ -4112,7 +4097,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D225" s="9">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E225" s="6">
         <v>322</v>
@@ -4123,7 +4108,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D226" s="9">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E226" s="6">
         <v>403</v>
@@ -4134,7 +4119,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D227" s="9">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E227" s="6">
         <v>404</v>
@@ -4145,7 +4130,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D228" s="9">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E228" s="6">
         <v>405</v>
@@ -4156,7 +4141,7 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D229" s="9">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E229" s="6">
         <v>409</v>
@@ -4227,7 +4212,7 @@
     <row r="237" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="238" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
@@ -4240,27 +4225,27 @@
         <v>0</v>
       </c>
       <c r="B239" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C239" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C239" s="13" t="s">
+      <c r="D239" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D239" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="E239" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F239" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="F239" s="12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="9">
+        <v>105</v>
+      </c>
+      <c r="B240" s="9">
         <v>104</v>
-      </c>
-      <c r="B240" s="9">
-        <v>111</v>
       </c>
       <c r="C240" s="9">
         <v>104</v>
@@ -4277,13 +4262,13 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="9">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B241" s="9">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C241" s="9">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D241" s="6">
         <v>105</v>
@@ -4297,10 +4282,10 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="9">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B242" s="9">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C242" s="9">
         <v>112</v>
@@ -4317,10 +4302,10 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="9">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B243" s="9">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="C243" s="9">
         <v>117</v>
@@ -4337,10 +4322,10 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="9">
+        <v>151</v>
+      </c>
+      <c r="B244" s="9">
         <v>122</v>
-      </c>
-      <c r="B244" s="9">
-        <v>152</v>
       </c>
       <c r="C244" s="9">
         <v>122</v>
@@ -4357,10 +4342,10 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="9">
+        <v>152</v>
+      </c>
+      <c r="B245" s="9">
         <v>123</v>
-      </c>
-      <c r="B245" s="9">
-        <v>153</v>
       </c>
       <c r="C245" s="9">
         <v>123</v>
@@ -4377,10 +4362,10 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="9">
+        <v>153</v>
+      </c>
+      <c r="B246" s="9">
         <v>151</v>
-      </c>
-      <c r="B246" s="9">
-        <v>154</v>
       </c>
       <c r="C246" s="9">
         <v>151</v>
@@ -4397,10 +4382,10 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="9">
+        <v>200</v>
+      </c>
+      <c r="B247" s="9">
         <v>152</v>
-      </c>
-      <c r="B247" s="9">
-        <v>200</v>
       </c>
       <c r="C247" s="9">
         <v>152</v>
@@ -4417,10 +4402,10 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="9">
+        <v>201</v>
+      </c>
+      <c r="B248" s="9">
         <v>153</v>
-      </c>
-      <c r="B248" s="9">
-        <v>201</v>
       </c>
       <c r="C248" s="9">
         <v>153</v>
@@ -4437,13 +4422,13 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="9">
+        <v>202</v>
+      </c>
+      <c r="B249" s="9">
         <v>154</v>
       </c>
-      <c r="B249" s="9">
-        <v>202</v>
-      </c>
       <c r="C249" s="9">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="D249" s="6">
         <v>123</v>
@@ -4457,13 +4442,13 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="9">
+        <v>203</v>
+      </c>
+      <c r="B250" s="9">
         <v>200</v>
       </c>
-      <c r="B250" s="9">
-        <v>204</v>
-      </c>
       <c r="C250" s="9">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D250" s="6">
         <v>151</v>
@@ -4477,13 +4462,13 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="9">
+        <v>204</v>
+      </c>
+      <c r="B251" s="9">
         <v>201</v>
       </c>
-      <c r="B251" s="9">
-        <v>206</v>
-      </c>
       <c r="C251" s="9">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D251" s="6">
         <v>152</v>
@@ -4497,13 +4482,13 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="9">
+        <v>206</v>
+      </c>
+      <c r="B252" s="9">
+        <v>203</v>
+      </c>
+      <c r="C252" s="9">
         <v>202</v>
-      </c>
-      <c r="B252" s="9">
-        <v>208</v>
-      </c>
-      <c r="C252" s="9">
-        <v>203</v>
       </c>
       <c r="D252" s="6">
         <v>153</v>
@@ -4517,10 +4502,10 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="9">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B253" s="9">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C253" s="9">
         <v>204</v>
@@ -4537,13 +4522,13 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="9">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B254" s="9">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C254" s="9">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D254" s="6">
         <v>200</v>
@@ -4557,13 +4542,13 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="9">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B255" s="9">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C255" s="9">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D255" s="6">
         <v>201</v>
@@ -4577,13 +4562,13 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="9">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B256" s="9">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C256" s="9">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D256" s="6">
         <v>202</v>
@@ -4597,13 +4582,13 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="9">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B257" s="9">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C257" s="9">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D257" s="6">
         <v>203</v>
@@ -4617,13 +4602,13 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="9">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B258" s="9">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C258" s="9">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D258" s="6">
         <v>204</v>
@@ -4637,13 +4622,13 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="9">
+        <v>215</v>
+      </c>
+      <c r="B259" s="9">
         <v>213</v>
       </c>
-      <c r="B259" s="9">
-        <v>219</v>
-      </c>
       <c r="C259" s="9">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D259" s="6">
         <v>206</v>
@@ -4657,13 +4642,13 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="9">
+        <v>216</v>
+      </c>
+      <c r="B260" s="9">
+        <v>214</v>
+      </c>
+      <c r="C260" s="9">
         <v>215</v>
-      </c>
-      <c r="B260" s="9">
-        <v>301</v>
-      </c>
-      <c r="C260" s="9">
-        <v>214</v>
       </c>
       <c r="D260" s="6">
         <v>208</v>
@@ -4677,10 +4662,10 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="9">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B261" s="9">
-        <v>302</v>
+        <v>215</v>
       </c>
       <c r="C261" s="9">
         <v>216</v>
@@ -4697,10 +4682,10 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="9">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B262" s="9">
-        <v>303</v>
+        <v>216</v>
       </c>
       <c r="C262" s="9">
         <v>217</v>
@@ -4717,10 +4702,10 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="9">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B263" s="9">
-        <v>304</v>
+        <v>217</v>
       </c>
       <c r="C263" s="9">
         <v>218</v>
@@ -4740,7 +4725,7 @@
         <v>301</v>
       </c>
       <c r="B264" s="9">
-        <v>305</v>
+        <v>218</v>
       </c>
       <c r="C264" s="9">
         <v>219</v>
@@ -4760,7 +4745,7 @@
         <v>303</v>
       </c>
       <c r="B265" s="9">
-        <v>306</v>
+        <v>219</v>
       </c>
       <c r="C265" s="9">
         <v>301</v>
@@ -4777,13 +4762,13 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="9">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B266" s="9">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C266" s="9">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D266" s="6">
         <v>215</v>
@@ -4797,13 +4782,13 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="9">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B267" s="9">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C267" s="9">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D267" s="6">
         <v>216</v>
@@ -4817,13 +4802,13 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="9">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B268" s="9">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="C268" s="9">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D268" s="6">
         <v>217</v>
@@ -4837,13 +4822,13 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="9">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B269" s="9">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="C269" s="9">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D269" s="6">
         <v>218</v>
@@ -4857,13 +4842,13 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="9">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B270" s="9">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="C270" s="9">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D270" s="6">
         <v>219</v>
@@ -4877,13 +4862,13 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="9">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B271" s="9">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C271" s="9">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D271" s="6">
         <v>301</v>
@@ -4897,13 +4882,13 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="9">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B272" s="9">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="C272" s="9">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D272" s="6">
         <v>302</v>
@@ -4917,13 +4902,13 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="9">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B273" s="9">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C273" s="9">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D273" s="6">
         <v>303</v>
@@ -4937,10 +4922,10 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="9">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B274" s="9">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C274" s="9">
         <v>317</v>
@@ -4960,7 +4945,7 @@
         <v>403</v>
       </c>
       <c r="B275" s="9">
-        <v>403</v>
+        <v>318</v>
       </c>
       <c r="C275" s="9">
         <v>319</v>
@@ -4980,7 +4965,7 @@
         <v>404</v>
       </c>
       <c r="B276" s="9">
-        <v>404</v>
+        <v>319</v>
       </c>
       <c r="C276" s="9">
         <v>321</v>
@@ -5000,7 +4985,7 @@
         <v>409</v>
       </c>
       <c r="B277" s="9">
-        <v>409</v>
+        <v>321</v>
       </c>
       <c r="C277" s="9">
         <v>322</v>
@@ -5020,7 +5005,7 @@
         <v>411</v>
       </c>
       <c r="B278" s="9">
-        <v>412</v>
+        <v>322</v>
       </c>
       <c r="C278" s="9">
         <v>403</v>
@@ -5035,12 +5020,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="279" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="10">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="9">
         <v>412</v>
       </c>
       <c r="B279" s="9">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="C279" s="9">
         <v>404</v>
@@ -5056,11 +5041,14 @@
       </c>
     </row>
     <row r="280" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B280" s="10">
-        <v>717</v>
+      <c r="A280" s="10">
+        <v>413</v>
+      </c>
+      <c r="B280" s="9">
+        <v>411</v>
       </c>
       <c r="C280" s="9">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D280" s="6">
         <v>314</v>
@@ -5072,9 +5060,12 @@
         <v>314</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B281" s="10">
+        <v>412</v>
+      </c>
       <c r="C281" s="9">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D281" s="6">
         <v>317</v>
@@ -5088,7 +5079,7 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C282" s="9">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D282" s="6">
         <v>318</v>

</xml_diff>